<commit_message>
Add BMCe data to EOL
</commit_message>
<xml_diff>
--- a/venv/EOL_data.xlsx
+++ b/venv/EOL_data.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FN2"/>
+  <dimension ref="A1:GA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,57 +432,57 @@
     <col width="11" customWidth="1" min="8" max="8"/>
     <col width="11" customWidth="1" min="9" max="9"/>
     <col width="13" customWidth="1" min="10" max="10"/>
-    <col width="14" customWidth="1" min="11" max="11"/>
-    <col width="14" customWidth="1" min="12" max="12"/>
-    <col width="16" customWidth="1" min="13" max="13"/>
-    <col width="13" customWidth="1" min="14" max="14"/>
-    <col width="9" customWidth="1" min="15" max="15"/>
-    <col width="9" customWidth="1" min="16" max="16"/>
-    <col width="9" customWidth="1" min="17" max="17"/>
-    <col width="9" customWidth="1" min="18" max="18"/>
-    <col width="9" customWidth="1" min="19" max="19"/>
-    <col width="9" customWidth="1" min="20" max="20"/>
-    <col width="9" customWidth="1" min="21" max="21"/>
-    <col width="9" customWidth="1" min="22" max="22"/>
-    <col width="9" customWidth="1" min="23" max="23"/>
-    <col width="10" customWidth="1" min="24" max="24"/>
-    <col width="10" customWidth="1" min="25" max="25"/>
-    <col width="10" customWidth="1" min="26" max="26"/>
-    <col width="10" customWidth="1" min="27" max="27"/>
-    <col width="10" customWidth="1" min="28" max="28"/>
-    <col width="10" customWidth="1" min="29" max="29"/>
-    <col width="10" customWidth="1" min="30" max="30"/>
-    <col width="10" customWidth="1" min="31" max="31"/>
-    <col width="10" customWidth="1" min="32" max="32"/>
-    <col width="10" customWidth="1" min="33" max="33"/>
-    <col width="10" customWidth="1" min="34" max="34"/>
-    <col width="10" customWidth="1" min="35" max="35"/>
-    <col width="10" customWidth="1" min="36" max="36"/>
+    <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="7" customWidth="1" min="12" max="12"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="14" max="14"/>
+    <col width="7" customWidth="1" min="15" max="15"/>
+    <col width="13" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+    <col width="11" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="16" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="21" max="21"/>
+    <col width="14" customWidth="1" min="22" max="22"/>
+    <col width="13" customWidth="1" min="23" max="23"/>
+    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="14" customWidth="1" min="25" max="25"/>
+    <col width="16" customWidth="1" min="26" max="26"/>
+    <col width="13" customWidth="1" min="27" max="27"/>
+    <col width="9" customWidth="1" min="28" max="28"/>
+    <col width="9" customWidth="1" min="29" max="29"/>
+    <col width="9" customWidth="1" min="30" max="30"/>
+    <col width="9" customWidth="1" min="31" max="31"/>
+    <col width="9" customWidth="1" min="32" max="32"/>
+    <col width="9" customWidth="1" min="33" max="33"/>
+    <col width="9" customWidth="1" min="34" max="34"/>
+    <col width="9" customWidth="1" min="35" max="35"/>
+    <col width="9" customWidth="1" min="36" max="36"/>
     <col width="10" customWidth="1" min="37" max="37"/>
     <col width="10" customWidth="1" min="38" max="38"/>
-    <col width="13" customWidth="1" min="39" max="39"/>
-    <col width="9" customWidth="1" min="40" max="40"/>
-    <col width="9" customWidth="1" min="41" max="41"/>
-    <col width="9" customWidth="1" min="42" max="42"/>
-    <col width="9" customWidth="1" min="43" max="43"/>
-    <col width="9" customWidth="1" min="44" max="44"/>
-    <col width="9" customWidth="1" min="45" max="45"/>
-    <col width="9" customWidth="1" min="46" max="46"/>
-    <col width="9" customWidth="1" min="47" max="47"/>
-    <col width="9" customWidth="1" min="48" max="48"/>
+    <col width="10" customWidth="1" min="39" max="39"/>
+    <col width="10" customWidth="1" min="40" max="40"/>
+    <col width="10" customWidth="1" min="41" max="41"/>
+    <col width="10" customWidth="1" min="42" max="42"/>
+    <col width="10" customWidth="1" min="43" max="43"/>
+    <col width="10" customWidth="1" min="44" max="44"/>
+    <col width="10" customWidth="1" min="45" max="45"/>
+    <col width="10" customWidth="1" min="46" max="46"/>
+    <col width="10" customWidth="1" min="47" max="47"/>
+    <col width="10" customWidth="1" min="48" max="48"/>
     <col width="10" customWidth="1" min="49" max="49"/>
     <col width="10" customWidth="1" min="50" max="50"/>
     <col width="10" customWidth="1" min="51" max="51"/>
-    <col width="10" customWidth="1" min="52" max="52"/>
-    <col width="10" customWidth="1" min="53" max="53"/>
-    <col width="10" customWidth="1" min="54" max="54"/>
-    <col width="10" customWidth="1" min="55" max="55"/>
-    <col width="10" customWidth="1" min="56" max="56"/>
-    <col width="10" customWidth="1" min="57" max="57"/>
-    <col width="10" customWidth="1" min="58" max="58"/>
-    <col width="10" customWidth="1" min="59" max="59"/>
-    <col width="10" customWidth="1" min="60" max="60"/>
-    <col width="10" customWidth="1" min="61" max="61"/>
+    <col width="13" customWidth="1" min="52" max="52"/>
+    <col width="9" customWidth="1" min="53" max="53"/>
+    <col width="9" customWidth="1" min="54" max="54"/>
+    <col width="9" customWidth="1" min="55" max="55"/>
+    <col width="9" customWidth="1" min="56" max="56"/>
+    <col width="9" customWidth="1" min="57" max="57"/>
+    <col width="9" customWidth="1" min="58" max="58"/>
+    <col width="9" customWidth="1" min="59" max="59"/>
+    <col width="9" customWidth="1" min="60" max="60"/>
+    <col width="9" customWidth="1" min="61" max="61"/>
     <col width="10" customWidth="1" min="62" max="62"/>
     <col width="10" customWidth="1" min="63" max="63"/>
     <col width="10" customWidth="1" min="64" max="64"/>
@@ -557,41 +557,54 @@
     <col width="10" customWidth="1" min="133" max="133"/>
     <col width="10" customWidth="1" min="134" max="134"/>
     <col width="10" customWidth="1" min="135" max="135"/>
-    <col width="13" customWidth="1" min="136" max="136"/>
-    <col width="7" customWidth="1" min="137" max="137"/>
-    <col width="7" customWidth="1" min="138" max="138"/>
-    <col width="7" customWidth="1" min="139" max="139"/>
-    <col width="7" customWidth="1" min="140" max="140"/>
-    <col width="20" customWidth="1" min="141" max="141"/>
-    <col width="20" customWidth="1" min="142" max="142"/>
-    <col width="17" customWidth="1" min="143" max="143"/>
-    <col width="20" customWidth="1" min="144" max="144"/>
-    <col width="17" customWidth="1" min="145" max="145"/>
-    <col width="14" customWidth="1" min="146" max="146"/>
+    <col width="10" customWidth="1" min="136" max="136"/>
+    <col width="10" customWidth="1" min="137" max="137"/>
+    <col width="10" customWidth="1" min="138" max="138"/>
+    <col width="10" customWidth="1" min="139" max="139"/>
+    <col width="10" customWidth="1" min="140" max="140"/>
+    <col width="10" customWidth="1" min="141" max="141"/>
+    <col width="10" customWidth="1" min="142" max="142"/>
+    <col width="10" customWidth="1" min="143" max="143"/>
+    <col width="10" customWidth="1" min="144" max="144"/>
+    <col width="10" customWidth="1" min="145" max="145"/>
+    <col width="10" customWidth="1" min="146" max="146"/>
     <col width="10" customWidth="1" min="147" max="147"/>
     <col width="10" customWidth="1" min="148" max="148"/>
-    <col width="15" customWidth="1" min="149" max="149"/>
-    <col width="15" customWidth="1" min="150" max="150"/>
-    <col width="16" customWidth="1" min="151" max="151"/>
-    <col width="15" customWidth="1" min="152" max="152"/>
-    <col width="10" customWidth="1" min="153" max="153"/>
-    <col width="10" customWidth="1" min="154" max="154"/>
-    <col width="6" customWidth="1" min="155" max="155"/>
-    <col width="6" customWidth="1" min="156" max="156"/>
-    <col width="18" customWidth="1" min="157" max="157"/>
-    <col width="18" customWidth="1" min="158" max="158"/>
-    <col width="10" customWidth="1" min="159" max="159"/>
+    <col width="13" customWidth="1" min="149" max="149"/>
+    <col width="7" customWidth="1" min="150" max="150"/>
+    <col width="7" customWidth="1" min="151" max="151"/>
+    <col width="7" customWidth="1" min="152" max="152"/>
+    <col width="7" customWidth="1" min="153" max="153"/>
+    <col width="20" customWidth="1" min="154" max="154"/>
+    <col width="20" customWidth="1" min="155" max="155"/>
+    <col width="17" customWidth="1" min="156" max="156"/>
+    <col width="20" customWidth="1" min="157" max="157"/>
+    <col width="17" customWidth="1" min="158" max="158"/>
+    <col width="14" customWidth="1" min="159" max="159"/>
     <col width="10" customWidth="1" min="160" max="160"/>
     <col width="10" customWidth="1" min="161" max="161"/>
-    <col width="11" customWidth="1" min="162" max="162"/>
-    <col width="16" customWidth="1" min="163" max="163"/>
+    <col width="15" customWidth="1" min="162" max="162"/>
+    <col width="15" customWidth="1" min="163" max="163"/>
     <col width="16" customWidth="1" min="164" max="164"/>
-    <col width="11" customWidth="1" min="165" max="165"/>
-    <col width="16" customWidth="1" min="166" max="166"/>
-    <col width="17" customWidth="1" min="167" max="167"/>
-    <col width="23" customWidth="1" min="168" max="168"/>
-    <col width="12" customWidth="1" min="169" max="169"/>
-    <col width="7" customWidth="1" min="170" max="170"/>
+    <col width="15" customWidth="1" min="165" max="165"/>
+    <col width="10" customWidth="1" min="166" max="166"/>
+    <col width="10" customWidth="1" min="167" max="167"/>
+    <col width="6" customWidth="1" min="168" max="168"/>
+    <col width="6" customWidth="1" min="169" max="169"/>
+    <col width="18" customWidth="1" min="170" max="170"/>
+    <col width="18" customWidth="1" min="171" max="171"/>
+    <col width="10" customWidth="1" min="172" max="172"/>
+    <col width="10" customWidth="1" min="173" max="173"/>
+    <col width="10" customWidth="1" min="174" max="174"/>
+    <col width="11" customWidth="1" min="175" max="175"/>
+    <col width="16" customWidth="1" min="176" max="176"/>
+    <col width="16" customWidth="1" min="177" max="177"/>
+    <col width="11" customWidth="1" min="178" max="178"/>
+    <col width="16" customWidth="1" min="179" max="179"/>
+    <col width="17" customWidth="1" min="180" max="180"/>
+    <col width="23" customWidth="1" min="181" max="181"/>
+    <col width="12" customWidth="1" min="182" max="182"/>
+    <col width="7" customWidth="1" min="183" max="183"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -647,795 +660,860 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>SW_BMCe</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>SW_CMC1</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>SW_CMC2</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>SW_CMC3</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>SW_CMC4</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>BatConfigPSet</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>ThermoPSet</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>VehiclePSet</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>TargetMarket</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>NameTargetMarket</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>NameVehiclePSet</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>NameThermoPSet</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>NameBatConfig</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
           <t>CellVoltageMin</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>CellVoltageMax</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>CellVoltageRange</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>CellTempCheck</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>CellTemp1</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>CellTemp2</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>CellTemp3</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>CellTemp4</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>CellTemp5</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>CellTemp6</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>CellTemp7</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>CellTemp8</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>CellTemp9</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>CellTemp10</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>CellTemp11</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>CellTemp12</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>CellTemp13</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>CellTemp14</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>CellTemp15</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>CellTemp16</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>CellTemp17</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>CellTemp18</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>CellTemp19</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>CellTemp20</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>CellTemp21</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>CellTemp22</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>CellTemp23</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>CellTemp24</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>CellTempRange</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>CellVolt1</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>CellVolt2</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>CellVolt3</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>CellVolt4</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>CellVolt5</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>CellVolt6</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>CellVolt7</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>CellVolt8</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>CellVolt9</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>CellVolt10</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>CellVolt11</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>CellVolt12</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>CellVolt13</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>CellVolt14</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>CellVolt15</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>CellVolt16</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>CellVolt17</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>CellVolt18</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>CellVolt19</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>CellVolt20</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BU1" t="inlineStr">
         <is>
           <t>CellVolt21</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BV1" t="inlineStr">
         <is>
           <t>CellVolt22</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BW1" t="inlineStr">
         <is>
           <t>CellVolt23</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BX1" t="inlineStr">
         <is>
           <t>CellVolt24</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BY1" t="inlineStr">
         <is>
           <t>CellVolt25</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BZ1" t="inlineStr">
         <is>
           <t>CellVolt26</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="CA1" t="inlineStr">
         <is>
           <t>CellVolt27</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>CellVolt28</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>CellVolt29</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>CellVolt30</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>CellVolt31</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>CellVolt32</t>
         </is>
       </c>
-      <c r="BT1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>CellVolt33</t>
         </is>
       </c>
-      <c r="BU1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>CellVolt34</t>
         </is>
       </c>
-      <c r="BV1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>CellVolt35</t>
         </is>
       </c>
-      <c r="BW1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>CellVolt36</t>
         </is>
       </c>
-      <c r="BX1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>CellVolt37</t>
         </is>
       </c>
-      <c r="BY1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>CellVolt38</t>
         </is>
       </c>
-      <c r="BZ1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>CellVolt39</t>
         </is>
       </c>
-      <c r="CA1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>CellVolt40</t>
         </is>
       </c>
-      <c r="CB1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>CellVolt41</t>
         </is>
       </c>
-      <c r="CC1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>CellVolt42</t>
         </is>
       </c>
-      <c r="CD1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>CellVolt43</t>
         </is>
       </c>
-      <c r="CE1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>CellVolt44</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>CellVolt45</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>CellVolt46</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>CellVolt47</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>CellVolt48</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>CellVolt49</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>CellVolt50</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>CellVolt51</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>CellVolt52</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>CellVolt53</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>CellVolt54</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>CellVolt55</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>CellVolt56</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>CellVolt57</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>CellVolt58</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>CellVolt59</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>CellVolt60</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>CellVolt61</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>CellVolt62</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>CellVolt63</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="DL1" t="inlineStr">
         <is>
           <t>CellVolt64</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DM1" t="inlineStr">
         <is>
           <t>CellVolt65</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DN1" t="inlineStr">
         <is>
           <t>CellVolt66</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DO1" t="inlineStr">
         <is>
           <t>CellVolt67</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DP1" t="inlineStr">
         <is>
           <t>CellVolt68</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DQ1" t="inlineStr">
         <is>
           <t>CellVolt69</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DR1" t="inlineStr">
         <is>
           <t>CellVolt70</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DS1" t="inlineStr">
         <is>
           <t>CellVolt71</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DT1" t="inlineStr">
         <is>
           <t>CellVolt72</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DU1" t="inlineStr">
         <is>
           <t>CellVolt73</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DV1" t="inlineStr">
         <is>
           <t>CellVolt74</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DW1" t="inlineStr">
         <is>
           <t>CellVolt75</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DX1" t="inlineStr">
         <is>
           <t>CellVolt76</t>
         </is>
       </c>
-      <c r="DL1" t="inlineStr">
+      <c r="DY1" t="inlineStr">
         <is>
           <t>CellVolt77</t>
         </is>
       </c>
-      <c r="DM1" t="inlineStr">
+      <c r="DZ1" t="inlineStr">
         <is>
           <t>CellVolt78</t>
         </is>
       </c>
-      <c r="DN1" t="inlineStr">
+      <c r="EA1" t="inlineStr">
         <is>
           <t>CellVolt79</t>
         </is>
       </c>
-      <c r="DO1" t="inlineStr">
+      <c r="EB1" t="inlineStr">
         <is>
           <t>CellVolt80</t>
         </is>
       </c>
-      <c r="DP1" t="inlineStr">
+      <c r="EC1" t="inlineStr">
         <is>
           <t>CellVolt81</t>
         </is>
       </c>
-      <c r="DQ1" t="inlineStr">
+      <c r="ED1" t="inlineStr">
         <is>
           <t>CellVolt82</t>
         </is>
       </c>
-      <c r="DR1" t="inlineStr">
+      <c r="EE1" t="inlineStr">
         <is>
           <t>CellVolt83</t>
         </is>
       </c>
-      <c r="DS1" t="inlineStr">
+      <c r="EF1" t="inlineStr">
         <is>
           <t>CellVolt84</t>
         </is>
       </c>
-      <c r="DT1" t="inlineStr">
+      <c r="EG1" t="inlineStr">
         <is>
           <t>CellVolt85</t>
         </is>
       </c>
-      <c r="DU1" t="inlineStr">
+      <c r="EH1" t="inlineStr">
         <is>
           <t>CellVolt86</t>
         </is>
       </c>
-      <c r="DV1" t="inlineStr">
+      <c r="EI1" t="inlineStr">
         <is>
           <t>CellVolt87</t>
         </is>
       </c>
-      <c r="DW1" t="inlineStr">
+      <c r="EJ1" t="inlineStr">
         <is>
           <t>CellVolt88</t>
         </is>
       </c>
-      <c r="DX1" t="inlineStr">
+      <c r="EK1" t="inlineStr">
         <is>
           <t>CellVolt89</t>
         </is>
       </c>
-      <c r="DY1" t="inlineStr">
+      <c r="EL1" t="inlineStr">
         <is>
           <t>CellVolt90</t>
         </is>
       </c>
-      <c r="DZ1" t="inlineStr">
+      <c r="EM1" t="inlineStr">
         <is>
           <t>CellVolt91</t>
         </is>
       </c>
-      <c r="EA1" t="inlineStr">
+      <c r="EN1" t="inlineStr">
         <is>
           <t>CellVolt92</t>
         </is>
       </c>
-      <c r="EB1" t="inlineStr">
+      <c r="EO1" t="inlineStr">
         <is>
           <t>CellVolt93</t>
         </is>
       </c>
-      <c r="EC1" t="inlineStr">
+      <c r="EP1" t="inlineStr">
         <is>
           <t>CellVolt94</t>
         </is>
       </c>
-      <c r="ED1" t="inlineStr">
+      <c r="EQ1" t="inlineStr">
         <is>
           <t>CellVolt95</t>
         </is>
       </c>
-      <c r="EE1" t="inlineStr">
+      <c r="ER1" t="inlineStr">
         <is>
           <t>CellVolt96</t>
         </is>
       </c>
-      <c r="EF1" t="inlineStr">
+      <c r="ES1" t="inlineStr">
         <is>
           <t>CellVoltRange</t>
         </is>
       </c>
-      <c r="EG1" t="inlineStr">
+      <c r="ET1" t="inlineStr">
         <is>
           <t>CV_DTC1</t>
         </is>
       </c>
-      <c r="EH1" t="inlineStr">
+      <c r="EU1" t="inlineStr">
         <is>
           <t>CV_DTC2</t>
         </is>
       </c>
-      <c r="EI1" t="inlineStr">
+      <c r="EV1" t="inlineStr">
         <is>
           <t>CV_DTC3</t>
         </is>
       </c>
-      <c r="EJ1" t="inlineStr">
+      <c r="EW1" t="inlineStr">
         <is>
           <t>CV_DTC4</t>
         </is>
       </c>
-      <c r="EK1" t="inlineStr">
+      <c r="EX1" t="inlineStr">
         <is>
           <t>CellVoltageMinActual</t>
         </is>
       </c>
-      <c r="EL1" t="inlineStr">
+      <c r="EY1" t="inlineStr">
         <is>
           <t>CellVoltageMaxActual</t>
         </is>
       </c>
-      <c r="EM1" t="inlineStr">
+      <c r="EZ1" t="inlineStr">
         <is>
           <t>CellTempMinActual</t>
         </is>
       </c>
-      <c r="EN1" t="inlineStr">
+      <c r="FA1" t="inlineStr">
         <is>
           <t>CellVoltageMaxActual</t>
         </is>
       </c>
-      <c r="EO1" t="inlineStr">
+      <c r="FB1" t="inlineStr">
         <is>
           <t>TempVoltageResult</t>
         </is>
       </c>
-      <c r="EP1" t="inlineStr">
+      <c r="FC1" t="inlineStr">
         <is>
           <t>PyroCheckCount</t>
         </is>
       </c>
-      <c r="EQ1" t="inlineStr">
+      <c r="FD1" t="inlineStr">
         <is>
           <t>PyroMinSet</t>
         </is>
       </c>
-      <c r="ER1" t="inlineStr">
+      <c r="FE1" t="inlineStr">
         <is>
           <t>PyroMaxSet</t>
         </is>
       </c>
-      <c r="ES1" t="inlineStr">
+      <c r="FF1" t="inlineStr">
         <is>
           <t>PyroCheckResult</t>
         </is>
       </c>
-      <c r="ET1" t="inlineStr">
+      <c r="FG1" t="inlineStr">
         <is>
           <t>PyroCheckStatus</t>
         </is>
       </c>
-      <c r="EU1" t="inlineStr">
+      <c r="FH1" t="inlineStr">
         <is>
           <t>Pilot Line Check</t>
         </is>
       </c>
-      <c r="EV1" t="inlineStr">
+      <c r="FI1" t="inlineStr">
         <is>
           <t>Klemme 30 Check</t>
         </is>
       </c>
-      <c r="EW1" t="inlineStr">
+      <c r="FJ1" t="inlineStr">
         <is>
           <t>R1 MBE Set</t>
         </is>
       </c>
-      <c r="EX1" t="inlineStr">
+      <c r="FK1" t="inlineStr">
         <is>
           <t>R2 MBE Set</t>
         </is>
       </c>
-      <c r="EY1" t="inlineStr">
+      <c r="FL1" t="inlineStr">
         <is>
           <t>R1 Set</t>
         </is>
       </c>
-      <c r="EZ1" t="inlineStr">
+      <c r="FM1" t="inlineStr">
         <is>
           <t>R2 Set</t>
         </is>
       </c>
-      <c r="FA1" t="inlineStr">
+      <c r="FN1" t="inlineStr">
         <is>
           <t>Iso Res 1 Setpoint</t>
         </is>
       </c>
-      <c r="FB1" t="inlineStr">
+      <c r="FO1" t="inlineStr">
         <is>
           <t>Iso Res 2 Setpoint</t>
         </is>
       </c>
-      <c r="FC1" t="inlineStr">
+      <c r="FP1" t="inlineStr">
         <is>
           <t>HV Min Iso</t>
         </is>
       </c>
-      <c r="FD1" t="inlineStr">
+      <c r="FQ1" t="inlineStr">
         <is>
           <t>HV Pos Iso</t>
         </is>
       </c>
-      <c r="FE1" t="inlineStr">
+      <c r="FR1" t="inlineStr">
         <is>
           <t>Iso Result</t>
         </is>
       </c>
-      <c r="FF1" t="inlineStr">
+      <c r="FS1" t="inlineStr">
         <is>
           <t>Voltage Set</t>
         </is>
       </c>
-      <c r="FG1" t="inlineStr">
+      <c r="FT1" t="inlineStr">
         <is>
           <t>Current Leak Min</t>
         </is>
       </c>
-      <c r="FH1" t="inlineStr">
+      <c r="FU1" t="inlineStr">
         <is>
           <t>Current Leak Max</t>
         </is>
       </c>
-      <c r="FI1" t="inlineStr">
+      <c r="FV1" t="inlineStr">
         <is>
           <t>Voltage Act</t>
         </is>
       </c>
-      <c r="FJ1" t="inlineStr">
+      <c r="FW1" t="inlineStr">
         <is>
           <t>Current Leak Act</t>
         </is>
       </c>
-      <c r="FK1" t="inlineStr">
+      <c r="FX1" t="inlineStr">
         <is>
           <t>Dielectric Result</t>
         </is>
       </c>
-      <c r="FL1" t="inlineStr">
+      <c r="FY1" t="inlineStr">
         <is>
           <t>Operating States Result</t>
         </is>
       </c>
-      <c r="FM1" t="inlineStr">
+      <c r="FZ1" t="inlineStr">
         <is>
           <t>Final Result</t>
         </is>
@@ -1494,568 +1572,564 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>1020</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0108</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>0107</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>0107</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>DEFAULTYYYYY</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>SK07810802K9</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>DEFAULTTHERM</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>62K108S2PSK0</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
           <t>2.50</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>4.20</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>50.00</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AN2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AR2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AS2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr">
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
+      <c r="BA2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="BB2" t="inlineStr">
         <is>
           <t>3.631</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="BC2" t="inlineStr">
         <is>
           <t>3.637</t>
         </is>
       </c>
-      <c r="AQ2" t="inlineStr">
+      <c r="BD2" t="inlineStr">
         <is>
           <t>3.631</t>
         </is>
       </c>
-      <c r="AR2" t="inlineStr">
+      <c r="BE2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
+      <c r="BF2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="AT2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="AU2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="AV2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="AW2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="AX2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="AZ2" t="inlineStr">
+      <c r="BG2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="BH2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="BJ2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="BK2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="BL2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="BM2" t="inlineStr">
         <is>
           <t>3.636</t>
         </is>
       </c>
-      <c r="BA2" t="inlineStr">
+      <c r="BN2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="BB2" t="inlineStr">
+      <c r="BO2" t="inlineStr">
         <is>
           <t>3.637</t>
         </is>
       </c>
-      <c r="BC2" t="inlineStr">
+      <c r="BP2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="BD2" t="inlineStr">
+      <c r="BQ2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BE2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="BF2" t="inlineStr">
+      <c r="BR2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="BS2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BG2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="BH2" t="inlineStr">
+      <c r="BT2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="BU2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BI2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="BJ2" t="inlineStr">
+      <c r="BV2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="BW2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BK2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="BL2" t="inlineStr">
+      <c r="BX2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="BY2" t="inlineStr">
         <is>
           <t>3.636</t>
         </is>
       </c>
-      <c r="BM2" t="inlineStr">
+      <c r="BZ2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="BN2" t="inlineStr">
+      <c r="CA2" t="inlineStr">
         <is>
           <t>3.637</t>
         </is>
       </c>
-      <c r="BO2" t="inlineStr">
+      <c r="CB2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="BP2" t="inlineStr">
+      <c r="CC2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BQ2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="BR2" t="inlineStr">
+      <c r="CD2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="CE2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BS2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="BT2" t="inlineStr">
+      <c r="CF2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="CG2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BU2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="BV2" t="inlineStr">
+      <c r="CH2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="CI2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="BW2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="BX2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="BY2" t="inlineStr">
+      <c r="CJ2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="CL2" t="inlineStr">
         <is>
           <t>3.631</t>
         </is>
       </c>
-      <c r="BZ2" t="inlineStr">
+      <c r="CM2" t="inlineStr">
         <is>
           <t>3.636</t>
         </is>
       </c>
-      <c r="CA2" t="inlineStr">
+      <c r="CN2" t="inlineStr">
         <is>
           <t>3.631</t>
         </is>
       </c>
-      <c r="CB2" t="inlineStr">
+      <c r="CO2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="CC2" t="inlineStr">
+      <c r="CP2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="CD2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CE2" t="inlineStr">
+      <c r="CQ2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="CR2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="CF2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CG2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CH2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CI2" t="inlineStr">
+      <c r="CS2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="CT2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="CU2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="CV2" t="inlineStr">
         <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="CJ2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CK2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CL2" t="inlineStr">
+      <c r="CW2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="CX2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="CY2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="CM2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CN2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CO2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CP2" t="inlineStr">
+      <c r="CZ2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="DA2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="DB2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="DC2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="CQ2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CR2" t="inlineStr">
+      <c r="DD2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DE2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="CS2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CT2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="CU2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CV2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CW2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CX2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CY2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="CZ2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DA2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DB2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DC2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DD2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DE2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
       <c r="DF2" t="inlineStr">
         <is>
-          <t>3.633</t>
+          <t>3.634</t>
         </is>
       </c>
       <c r="DG2" t="inlineStr">
         <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="DH2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DI2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DJ2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DK2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DL2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DM2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DN2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DO2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DP2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DQ2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DR2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DS2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="DT2" t="inlineStr">
+        <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="DH2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DI2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DJ2" t="inlineStr">
+      <c r="DU2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="DV2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="DW2" t="inlineStr">
         <is>
           <t>3.635</t>
         </is>
       </c>
-      <c r="DK2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DL2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DM2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DN2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DO2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DP2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DQ2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DR2" t="inlineStr">
-        <is>
-          <t>3.634</t>
-        </is>
-      </c>
-      <c r="DS2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DT2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DU2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DV2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="DW2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
       <c r="DX2" t="inlineStr">
         <is>
-          <t>3.633</t>
+          <t>3.634</t>
         </is>
       </c>
       <c r="DY2" t="inlineStr">
@@ -2065,47 +2139,99 @@
       </c>
       <c r="DZ2" t="inlineStr">
         <is>
-          <t>3.633</t>
+          <t>3.634</t>
         </is>
       </c>
       <c r="EA2" t="inlineStr">
         <is>
-          <t>3.633</t>
+          <t>3.634</t>
         </is>
       </c>
       <c r="EB2" t="inlineStr">
         <is>
-          <t>3.633</t>
+          <t>3.634</t>
         </is>
       </c>
       <c r="EC2" t="inlineStr">
         <is>
-          <t>3.633</t>
+          <t>3.634</t>
         </is>
       </c>
       <c r="ED2" t="inlineStr">
         <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="EE2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="EF2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EG2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EH2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EI2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EJ2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EK2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EL2" t="inlineStr">
+        <is>
+          <t>3.634</t>
+        </is>
+      </c>
+      <c r="EM2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EP2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
+      <c r="EQ2" t="inlineStr">
+        <is>
           <t>3.632</t>
         </is>
       </c>
-      <c r="EE2" t="inlineStr">
-        <is>
-          <t>3.633</t>
-        </is>
-      </c>
-      <c r="EF2" t="inlineStr"/>
-      <c r="EG2" t="inlineStr"/>
-      <c r="EH2" t="inlineStr"/>
-      <c r="EI2" t="inlineStr"/>
-      <c r="EJ2" t="inlineStr"/>
-      <c r="EK2" t="inlineStr"/>
-      <c r="EL2" t="inlineStr"/>
-      <c r="EM2" t="inlineStr"/>
-      <c r="EN2" t="inlineStr"/>
-      <c r="EO2" t="inlineStr"/>
-      <c r="EP2" t="inlineStr"/>
-      <c r="EQ2" t="inlineStr"/>
-      <c r="ER2" t="inlineStr"/>
+      <c r="ER2" t="inlineStr">
+        <is>
+          <t>3.633</t>
+        </is>
+      </c>
       <c r="ES2" t="inlineStr"/>
       <c r="ET2" t="inlineStr"/>
       <c r="EU2" t="inlineStr"/>
@@ -2119,43 +2245,56 @@
       <c r="FC2" t="inlineStr"/>
       <c r="FD2" t="inlineStr"/>
       <c r="FE2" t="inlineStr"/>
-      <c r="FF2" t="inlineStr">
+      <c r="FF2" t="inlineStr"/>
+      <c r="FG2" t="inlineStr"/>
+      <c r="FH2" t="inlineStr"/>
+      <c r="FI2" t="inlineStr"/>
+      <c r="FJ2" t="inlineStr"/>
+      <c r="FK2" t="inlineStr"/>
+      <c r="FL2" t="inlineStr"/>
+      <c r="FM2" t="inlineStr"/>
+      <c r="FN2" t="inlineStr"/>
+      <c r="FO2" t="inlineStr"/>
+      <c r="FP2" t="inlineStr"/>
+      <c r="FQ2" t="inlineStr"/>
+      <c r="FR2" t="inlineStr"/>
+      <c r="FS2" t="inlineStr">
         <is>
           <t>2150.00</t>
         </is>
       </c>
-      <c r="FG2" t="inlineStr">
+      <c r="FT2" t="inlineStr">
         <is>
           <t>1.00</t>
         </is>
       </c>
-      <c r="FH2" t="inlineStr">
+      <c r="FU2" t="inlineStr">
         <is>
           <t>5.00</t>
         </is>
       </c>
-      <c r="FI2" t="inlineStr">
+      <c r="FV2" t="inlineStr">
         <is>
           <t>2151.00</t>
         </is>
       </c>
-      <c r="FJ2" t="inlineStr">
+      <c r="FW2" t="inlineStr">
         <is>
           <t>1.70</t>
         </is>
       </c>
-      <c r="FK2" t="inlineStr">
+      <c r="FX2" t="inlineStr">
         <is>
           <t>"IO"</t>
         </is>
       </c>
-      <c r="FL2" t="inlineStr"/>
-      <c r="FM2" t="inlineStr">
+      <c r="FY2" t="inlineStr"/>
+      <c r="FZ2" t="inlineStr">
         <is>
           <t>"IO"</t>
         </is>
       </c>
-      <c r="FN2" t="inlineStr">
+      <c r="GA2" t="inlineStr">
         <is>
           <t>EOL.ini</t>
         </is>

</xml_diff>

<commit_message>
Bug Fix - CellTempMaxActual
</commit_message>
<xml_diff>
--- a/venv/EOL_data.xlsx
+++ b/venv/EOL_data.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:GA2"/>
+  <dimension ref="A1:FW2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,40 +571,36 @@
     <col width="10" customWidth="1" min="147" max="147"/>
     <col width="10" customWidth="1" min="148" max="148"/>
     <col width="13" customWidth="1" min="149" max="149"/>
-    <col width="7" customWidth="1" min="150" max="150"/>
-    <col width="7" customWidth="1" min="151" max="151"/>
-    <col width="7" customWidth="1" min="152" max="152"/>
-    <col width="7" customWidth="1" min="153" max="153"/>
-    <col width="20" customWidth="1" min="154" max="154"/>
-    <col width="20" customWidth="1" min="155" max="155"/>
-    <col width="17" customWidth="1" min="156" max="156"/>
-    <col width="20" customWidth="1" min="157" max="157"/>
-    <col width="17" customWidth="1" min="158" max="158"/>
-    <col width="14" customWidth="1" min="159" max="159"/>
-    <col width="10" customWidth="1" min="160" max="160"/>
-    <col width="10" customWidth="1" min="161" max="161"/>
-    <col width="15" customWidth="1" min="162" max="162"/>
-    <col width="15" customWidth="1" min="163" max="163"/>
-    <col width="16" customWidth="1" min="164" max="164"/>
-    <col width="15" customWidth="1" min="165" max="165"/>
-    <col width="10" customWidth="1" min="166" max="166"/>
-    <col width="10" customWidth="1" min="167" max="167"/>
-    <col width="6" customWidth="1" min="168" max="168"/>
-    <col width="6" customWidth="1" min="169" max="169"/>
-    <col width="18" customWidth="1" min="170" max="170"/>
-    <col width="18" customWidth="1" min="171" max="171"/>
-    <col width="10" customWidth="1" min="172" max="172"/>
-    <col width="10" customWidth="1" min="173" max="173"/>
-    <col width="10" customWidth="1" min="174" max="174"/>
-    <col width="11" customWidth="1" min="175" max="175"/>
-    <col width="16" customWidth="1" min="176" max="176"/>
-    <col width="16" customWidth="1" min="177" max="177"/>
-    <col width="11" customWidth="1" min="178" max="178"/>
-    <col width="16" customWidth="1" min="179" max="179"/>
-    <col width="17" customWidth="1" min="180" max="180"/>
-    <col width="23" customWidth="1" min="181" max="181"/>
-    <col width="12" customWidth="1" min="182" max="182"/>
-    <col width="7" customWidth="1" min="183" max="183"/>
+    <col width="20" customWidth="1" min="150" max="150"/>
+    <col width="20" customWidth="1" min="151" max="151"/>
+    <col width="17" customWidth="1" min="152" max="152"/>
+    <col width="20" customWidth="1" min="153" max="153"/>
+    <col width="17" customWidth="1" min="154" max="154"/>
+    <col width="14" customWidth="1" min="155" max="155"/>
+    <col width="10" customWidth="1" min="156" max="156"/>
+    <col width="10" customWidth="1" min="157" max="157"/>
+    <col width="15" customWidth="1" min="158" max="158"/>
+    <col width="15" customWidth="1" min="159" max="159"/>
+    <col width="16" customWidth="1" min="160" max="160"/>
+    <col width="15" customWidth="1" min="161" max="161"/>
+    <col width="10" customWidth="1" min="162" max="162"/>
+    <col width="10" customWidth="1" min="163" max="163"/>
+    <col width="6" customWidth="1" min="164" max="164"/>
+    <col width="6" customWidth="1" min="165" max="165"/>
+    <col width="18" customWidth="1" min="166" max="166"/>
+    <col width="18" customWidth="1" min="167" max="167"/>
+    <col width="10" customWidth="1" min="168" max="168"/>
+    <col width="10" customWidth="1" min="169" max="169"/>
+    <col width="10" customWidth="1" min="170" max="170"/>
+    <col width="11" customWidth="1" min="171" max="171"/>
+    <col width="16" customWidth="1" min="172" max="172"/>
+    <col width="16" customWidth="1" min="173" max="173"/>
+    <col width="11" customWidth="1" min="174" max="174"/>
+    <col width="16" customWidth="1" min="175" max="175"/>
+    <col width="17" customWidth="1" min="176" max="176"/>
+    <col width="23" customWidth="1" min="177" max="177"/>
+    <col width="12" customWidth="1" min="178" max="178"/>
+    <col width="7" customWidth="1" min="179" max="179"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1355,165 +1351,145 @@
       </c>
       <c r="ET1" t="inlineStr">
         <is>
-          <t>CV_DTC1</t>
+          <t>CellVoltageMinActual</t>
         </is>
       </c>
       <c r="EU1" t="inlineStr">
         <is>
-          <t>CV_DTC2</t>
+          <t>CellVoltageMaxActual</t>
         </is>
       </c>
       <c r="EV1" t="inlineStr">
         <is>
-          <t>CV_DTC3</t>
+          <t>CellTempMinActual</t>
         </is>
       </c>
       <c r="EW1" t="inlineStr">
         <is>
-          <t>CV_DTC4</t>
+          <t>CellVoltageMaxActual</t>
         </is>
       </c>
       <c r="EX1" t="inlineStr">
         <is>
-          <t>CellVoltageMinActual</t>
+          <t>TempVoltageResult</t>
         </is>
       </c>
       <c r="EY1" t="inlineStr">
         <is>
-          <t>CellVoltageMaxActual</t>
+          <t>PyroCheckCount</t>
         </is>
       </c>
       <c r="EZ1" t="inlineStr">
         <is>
-          <t>CellTempMinActual</t>
+          <t>PyroMinSet</t>
         </is>
       </c>
       <c r="FA1" t="inlineStr">
         <is>
-          <t>CellVoltageMaxActual</t>
+          <t>PyroMaxSet</t>
         </is>
       </c>
       <c r="FB1" t="inlineStr">
         <is>
-          <t>TempVoltageResult</t>
+          <t>PyroCheckResult</t>
         </is>
       </c>
       <c r="FC1" t="inlineStr">
         <is>
-          <t>PyroCheckCount</t>
+          <t>PyroCheckStatus</t>
         </is>
       </c>
       <c r="FD1" t="inlineStr">
         <is>
-          <t>PyroMinSet</t>
+          <t>Pilot Line Check</t>
         </is>
       </c>
       <c r="FE1" t="inlineStr">
         <is>
-          <t>PyroMaxSet</t>
+          <t>Klemme 30 Check</t>
         </is>
       </c>
       <c r="FF1" t="inlineStr">
         <is>
-          <t>PyroCheckResult</t>
+          <t>R1 MBE Set</t>
         </is>
       </c>
       <c r="FG1" t="inlineStr">
         <is>
-          <t>PyroCheckStatus</t>
+          <t>R2 MBE Set</t>
         </is>
       </c>
       <c r="FH1" t="inlineStr">
         <is>
-          <t>Pilot Line Check</t>
+          <t>R1 Set</t>
         </is>
       </c>
       <c r="FI1" t="inlineStr">
         <is>
-          <t>Klemme 30 Check</t>
+          <t>R2 Set</t>
         </is>
       </c>
       <c r="FJ1" t="inlineStr">
         <is>
-          <t>R1 MBE Set</t>
+          <t>Iso Res 1 Setpoint</t>
         </is>
       </c>
       <c r="FK1" t="inlineStr">
         <is>
-          <t>R2 MBE Set</t>
+          <t>Iso Res 2 Setpoint</t>
         </is>
       </c>
       <c r="FL1" t="inlineStr">
         <is>
-          <t>R1 Set</t>
+          <t>HV Min Iso</t>
         </is>
       </c>
       <c r="FM1" t="inlineStr">
         <is>
-          <t>R2 Set</t>
+          <t>HV Pos Iso</t>
         </is>
       </c>
       <c r="FN1" t="inlineStr">
         <is>
-          <t>Iso Res 1 Setpoint</t>
+          <t>Iso Result</t>
         </is>
       </c>
       <c r="FO1" t="inlineStr">
         <is>
-          <t>Iso Res 2 Setpoint</t>
+          <t>Voltage Set</t>
         </is>
       </c>
       <c r="FP1" t="inlineStr">
         <is>
-          <t>HV Min Iso</t>
+          <t>Current Leak Min</t>
         </is>
       </c>
       <c r="FQ1" t="inlineStr">
         <is>
-          <t>HV Pos Iso</t>
+          <t>Current Leak Max</t>
         </is>
       </c>
       <c r="FR1" t="inlineStr">
         <is>
-          <t>Iso Result</t>
+          <t>Voltage Act</t>
         </is>
       </c>
       <c r="FS1" t="inlineStr">
         <is>
-          <t>Voltage Set</t>
+          <t>Current Leak Act</t>
         </is>
       </c>
       <c r="FT1" t="inlineStr">
         <is>
-          <t>Current Leak Min</t>
+          <t>Dielectric Result</t>
         </is>
       </c>
       <c r="FU1" t="inlineStr">
         <is>
-          <t>Current Leak Max</t>
+          <t>Operating States Result</t>
         </is>
       </c>
       <c r="FV1" t="inlineStr">
-        <is>
-          <t>Voltage Act</t>
-        </is>
-      </c>
-      <c r="FW1" t="inlineStr">
-        <is>
-          <t>Current Leak Act</t>
-        </is>
-      </c>
-      <c r="FX1" t="inlineStr">
-        <is>
-          <t>Dielectric Result</t>
-        </is>
-      </c>
-      <c r="FY1" t="inlineStr">
-        <is>
-          <t>Operating States Result</t>
-        </is>
-      </c>
-      <c r="FZ1" t="inlineStr">
         <is>
           <t>Final Result</t>
         </is>
@@ -2232,12 +2208,36 @@
           <t>3.633</t>
         </is>
       </c>
-      <c r="ES2" t="inlineStr"/>
-      <c r="ET2" t="inlineStr"/>
-      <c r="EU2" t="inlineStr"/>
-      <c r="EV2" t="inlineStr"/>
-      <c r="EW2" t="inlineStr"/>
-      <c r="EX2" t="inlineStr"/>
+      <c r="ES2" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="ET2" t="inlineStr">
+        <is>
+          <t>3.631</t>
+        </is>
+      </c>
+      <c r="EU2" t="inlineStr">
+        <is>
+          <t>3.635</t>
+        </is>
+      </c>
+      <c r="EV2" t="inlineStr">
+        <is>
+          <t>22.500</t>
+        </is>
+      </c>
+      <c r="EW2" t="inlineStr">
+        <is>
+          <t>3.635</t>
+        </is>
+      </c>
+      <c r="EX2" t="inlineStr">
+        <is>
+          <t>"IO"</t>
+        </is>
+      </c>
       <c r="EY2" t="inlineStr"/>
       <c r="EZ2" t="inlineStr"/>
       <c r="FA2" t="inlineStr"/>
@@ -2254,47 +2254,43 @@
       <c r="FL2" t="inlineStr"/>
       <c r="FM2" t="inlineStr"/>
       <c r="FN2" t="inlineStr"/>
-      <c r="FO2" t="inlineStr"/>
-      <c r="FP2" t="inlineStr"/>
-      <c r="FQ2" t="inlineStr"/>
-      <c r="FR2" t="inlineStr"/>
+      <c r="FO2" t="inlineStr">
+        <is>
+          <t>2150.00</t>
+        </is>
+      </c>
+      <c r="FP2" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="FQ2" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="FR2" t="inlineStr">
+        <is>
+          <t>2151.00</t>
+        </is>
+      </c>
       <c r="FS2" t="inlineStr">
         <is>
-          <t>2150.00</t>
+          <t>1.70</t>
         </is>
       </c>
       <c r="FT2" t="inlineStr">
         <is>
-          <t>1.00</t>
-        </is>
-      </c>
-      <c r="FU2" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
+          <t>"IO"</t>
+        </is>
+      </c>
+      <c r="FU2" t="inlineStr"/>
       <c r="FV2" t="inlineStr">
         <is>
-          <t>2151.00</t>
+          <t>"IO"</t>
         </is>
       </c>
       <c r="FW2" t="inlineStr">
-        <is>
-          <t>1.70</t>
-        </is>
-      </c>
-      <c r="FX2" t="inlineStr">
-        <is>
-          <t>"IO"</t>
-        </is>
-      </c>
-      <c r="FY2" t="inlineStr"/>
-      <c r="FZ2" t="inlineStr">
-        <is>
-          <t>"IO"</t>
-        </is>
-      </c>
-      <c r="GA2" t="inlineStr">
         <is>
           <t>EOL.ini</t>
         </is>

</xml_diff>